<commit_message>
fix: replace Zm langs options with SA lang opts (#1157)
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/contact/person-edit.xlsx
+++ b/config/itech-aurum/forms/contact/person-edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/contact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C470638-1092-E748-96F7-10F0E7F24BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802AFBBD-8D8C-7D49-8D27-12FDD06C9A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,12 +86,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>shona</t>
-  </si>
-  <si>
-    <t>Shona</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -203,12 +197,6 @@
     <t>end group</t>
   </si>
   <si>
-    <t>ndebele</t>
-  </si>
-  <si>
-    <t>Ndebele</t>
-  </si>
-  <si>
     <t>db:health_center</t>
   </si>
   <si>
@@ -276,6 +264,18 @@
   </si>
   <si>
     <t>${age} &gt;= 15 and ${age} &lt;= 75</t>
+  </si>
+  <si>
+    <t>afrikaans</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>setswana</t>
+  </si>
+  <si>
+    <t>Setswana</t>
   </si>
 </sst>
 </file>
@@ -705,9 +705,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -757,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -813,22 +813,22 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -851,21 +851,21 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>13</v>
@@ -891,26 +891,26 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -934,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -965,20 +965,20 @@
     </row>
     <row r="7" spans="1:26" s="13" customFormat="1" ht="16">
       <c r="A7" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="8" spans="1:26" s="13" customFormat="1" ht="16">
       <c r="A8" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>1</v>
@@ -1011,7 +1011,7 @@
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
       <c r="E8" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="7"/>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="9" spans="1:26" s="13" customFormat="1" ht="16">
       <c r="A9" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="16"/>
@@ -1067,26 +1067,26 @@
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1107,26 +1107,26 @@
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1147,10 +1147,10 @@
     </row>
     <row r="12" spans="1:26" ht="17" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>14</v>
@@ -1162,7 +1162,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1182,10 +1182,10 @@
     </row>
     <row r="13" spans="1:26" ht="20" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>14</v>
@@ -1198,7 +1198,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -1218,20 +1218,20 @@
     </row>
     <row r="14" spans="1:26" ht="24" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1256,26 +1256,26 @@
     </row>
     <row r="15" spans="1:26" ht="16">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1296,26 +1296,26 @@
     </row>
     <row r="16" spans="1:26" ht="16">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1336,18 +1336,18 @@
     </row>
     <row r="17" spans="1:26" ht="16">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1372,26 +1372,26 @@
     </row>
     <row r="18" spans="1:26" ht="16">
       <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="19" spans="1:26" ht="16">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2707,7 +2707,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -2731,36 +2731,36 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="16">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>20</v>
+      <c r="B3" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="13" customFormat="1" ht="16">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>59</v>
+      <c r="B4" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -2788,13 +2788,13 @@
     </row>
     <row r="5" spans="1:26" s="13" customFormat="1" ht="18.75" customHeight="1">
       <c r="A5" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>78</v>
-      </c>
       <c r="C5" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2822,13 +2822,13 @@
     </row>
     <row r="6" spans="1:26" s="13" customFormat="1" ht="18.75" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -4248,16 +4248,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -4272,19 +4272,19 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="10">
         <v>43936</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>

</xml_diff>

<commit_message>
fix: edit contact vmmc no constrait fix: phone error message
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/contact/person-edit.xlsx
+++ b/config/itech-aurum/forms/contact/person-edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/contact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D93DB1-8026-484B-A6F7-FE282A387312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B2F1E4-7BA4-774B-AE96-E11BFD717FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1140" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-2900" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -161,9 +161,6 @@
     <t>Client Mobile phone number</t>
   </si>
   <si>
-    <t>Please enter phone number in the format +263xxxxxxxxx</t>
-  </si>
-  <si>
     <t>alternative_phone</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>enrolled_by</t>
+  </si>
+  <si>
+    <t>Please enter phone number in the format +27xxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -325,6 +325,7 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Proxima Nova"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -686,7 +687,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD9"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -736,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -926,7 +927,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>40</v>
@@ -953,10 +954,10 @@
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -966,10 +967,10 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -993,7 +994,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>14</v>
@@ -1005,7 +1006,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1025,10 +1026,10 @@
     </row>
     <row r="9" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>14</v>
@@ -1041,7 +1042,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1061,16 +1062,16 @@
     </row>
     <row r="10" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>64</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>65</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="14" t="s">
@@ -1115,10 +1116,10 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1142,23 +1143,23 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1179,13 +1180,13 @@
     </row>
     <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1215,13 +1216,13 @@
     </row>
     <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1255,7 +1256,7 @@
     </row>
     <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2589,10 +2590,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
@@ -2600,10 +2601,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>75</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -2634,10 +2635,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -2668,10 +2669,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>78</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>79</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -2727,13 +2728,13 @@
     </row>
     <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -2761,13 +2762,13 @@
     </row>
     <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>70</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>

</xml_diff>

<commit_message>
fix: contact file number regex
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/contact/person-edit.xlsx
+++ b/config/itech-aurum/forms/contact/person-edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/contact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B2F1E4-7BA4-774B-AE96-E11BFD717FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752CFD34-7EA9-B84D-9DAD-84E3E3BC53F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2900" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>VMMC Client Number</t>
   </si>
   <si>
-    <t>Must be 5 – 9 numeric digits</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -266,13 +263,16 @@
     <t>Zulu</t>
   </si>
   <si>
-    <t>regex(., '^[0-9a-zA-Z]{5,9}$')</t>
-  </si>
-  <si>
     <t>enrolled_by</t>
   </si>
   <si>
     <t>Please enter phone number in the format +27xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>regex(., '^[\w-]{5,9}$')</t>
+  </si>
+  <si>
+    <t>Must be 5 – 9 alpha-numeric characters, cannot have white spaces</t>
   </si>
 </sst>
 </file>
@@ -687,7 +687,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -737,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -927,10 +927,10 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -951,13 +951,13 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -967,10 +967,10 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -994,7 +994,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>14</v>
@@ -1006,7 +1006,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1026,10 +1026,10 @@
     </row>
     <row r="9" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>14</v>
@@ -1042,7 +1042,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1062,16 +1062,16 @@
     </row>
     <row r="10" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>63</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="14" t="s">
@@ -1103,10 +1103,10 @@
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1116,10 +1116,10 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1143,23 +1143,23 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1180,13 +1180,13 @@
     </row>
     <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1216,13 +1216,13 @@
     </row>
     <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2590,10 +2590,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
@@ -2601,10 +2601,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -2635,10 +2635,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -2669,10 +2669,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -2728,13 +2728,13 @@
     </row>
     <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -2762,13 +2762,13 @@
     </row>
     <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>69</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>

</xml_diff>